<commit_message>
Latest versions from Google Docs
Updated with latest versions from Google Docs, some modifications by anonymous and Mikko
</commit_message>
<xml_diff>
--- a/2017_Stockholm/Taxonomy_API_draft_2017-05-18.xlsx
+++ b/2017_Stockholm/Taxonomy_API_draft_2017-05-18.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t>Draft of taxonomy API standard</t>
   </si>
@@ -222,7 +222,9 @@
 /species/suggest</t>
   </si>
   <si>
-    <t>https://api.laji.fi/taxa/search *</t>
+    <t>https://api.laji.fi/taxa/search
+https://api.laji.fi/taxa/{id} *
+https://api.laji.fi/taxa/{id}/children **</t>
   </si>
   <si>
     <t>Returns taxon record(s). This API call can be used for autocomplete searches, matching searches (returns type of match among other things), etc by setting appropriate parameters. We suggest that search_type adheres to standardized terms used in e.g. Apache Lucene.
@@ -251,9 +253,6 @@
   </si>
   <si>
     <t>/api/taxonomy/taxon/{pk}/subtree</t>
-  </si>
-  <si>
-    <t>https://api.laji.fi/taxa/{id}/children **</t>
   </si>
   <si>
     <t>Returns the entire subtree rooted at the specified taxon. Is this the same as /api/taxonomy/taxon/?filter[ancestor]={taxon_id}? Does it return both taxa and related objects?</t>
@@ -938,10 +937,10 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="G25" s="16" t="s">
         <v>24</v>
@@ -950,38 +949,38 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="18"/>
       <c r="F26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="H26" s="7"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="18"/>
       <c r="F27" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>30</v>
@@ -990,20 +989,20 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>24</v>
@@ -1012,16 +1011,16 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="18"/>
       <c r="F29" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>30</v>
@@ -1030,20 +1029,20 @@
     </row>
     <row r="30">
       <c r="A30" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="C30" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>24</v>
@@ -1052,10 +1051,10 @@
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>37</v>
@@ -1065,7 +1064,7 @@
         <v>27</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>24</v>
@@ -1074,10 +1073,10 @@
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>37</v>
@@ -1085,18 +1084,18 @@
       <c r="D32" s="16"/>
       <c r="E32" s="18"/>
       <c r="F32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="H32" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="22"/>
       <c r="C33" s="21" t="s">
@@ -1107,13 +1106,13 @@
         <v>27</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>24</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
@@ -1139,7 +1138,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37">
@@ -1150,10 +1149,10 @@
         <v>13</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10" t="s">
@@ -1168,22 +1167,22 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>24</v>
@@ -1202,18 +1201,18 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="15"/>
       <c r="F40" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>24</v>
@@ -1221,18 +1220,18 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>24</v>
@@ -1240,19 +1239,19 @@
     </row>
     <row r="42">
       <c r="A42" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="H42" s="28"/>
     </row>
@@ -1268,7 +1267,7 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F44" s="8"/>
     </row>
@@ -1278,7 +1277,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F45" s="8"/>
     </row>
@@ -1288,7 +1287,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" s="8"/>
     </row>
@@ -1298,7 +1297,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -1308,7 +1307,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F48" s="8"/>
     </row>

</xml_diff>